<commit_message>
update acetyl supp data
</commit_message>
<xml_diff>
--- a/Supplementary data/CellCycle_Acetylation_Predictions.xlsx
+++ b/Supplementary data/CellCycle_Acetylation_Predictions.xlsx
@@ -1,28 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirksmi\Documents\GitHub\CAROM\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kirksmi\Documents\GitHub\CAROM\Supplementary data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{60C8C464-32FC-41E0-A2BB-C3F783DF3420}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04A26888-A13E-4FA2-8328-FCDB85ACEC55}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AcetylPred_AllPhases" sheetId="1" r:id="rId1"/>
     <sheet name="AcetylPred_Unique" sheetId="2" r:id="rId2"/>
     <sheet name="AcetylPred_DrugOverlap" sheetId="3" r:id="rId3"/>
+    <sheet name="DrugOverlap_Hypergeometric" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2127" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2146" uniqueCount="281">
   <si>
     <t>genes</t>
   </si>
@@ -811,13 +823,79 @@
   </si>
   <si>
     <t>PCI</t>
+  </si>
+  <si>
+    <t>Nicotinamide (45)</t>
+  </si>
+  <si>
+    <t>Tenovin-6 (73)</t>
+  </si>
+  <si>
+    <t>Tubacin (75)</t>
+  </si>
+  <si>
+    <t>PCI-24781 (59)</t>
+  </si>
+  <si>
+    <t>G0 (38)</t>
+  </si>
+  <si>
+    <t>G1 (35)</t>
+  </si>
+  <si>
+    <t>S (41)</t>
+  </si>
+  <si>
+    <t>G2 (82)</t>
+  </si>
+  <si>
+    <t>Pandacostat (5)</t>
+  </si>
+  <si>
+    <t>MGCD0103 (45)</t>
+  </si>
+  <si>
+    <t>NaButyrate (16)</t>
+  </si>
+  <si>
+    <t>Valproate (14)</t>
+  </si>
+  <si>
+    <r>
+      <t>Sirtinol</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> (10)</t>
+    </r>
+  </si>
+  <si>
+    <t>4.28 E-5</t>
+  </si>
+  <si>
+    <t>2.82 E-5</t>
+  </si>
+  <si>
+    <t>6.26 E-5</t>
+  </si>
+  <si>
+    <t>1.03 E-4</t>
+  </si>
+  <si>
+    <t>1.79 E-4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -952,8 +1030,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF191919"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF191919"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1133,8 +1244,14 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD8D8D8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1249,6 +1366,292 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF181818"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF181818"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF181818"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF181818"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF181818"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF181818"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF181818"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF181818"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF181818"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF181818"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF181818"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF181818"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF181818"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF181818"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF181818"/>
+      </left>
+      <right style="thick">
+        <color rgb="FF181818"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF181818"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF181818"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF181818"/>
+      </right>
+      <top style="thick">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF181818"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF181818"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF181818"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF181818"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF181818"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF181818"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF181818"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thick">
+        <color rgb="FF181818"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FF181818"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thick">
+        <color rgb="FF181818"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thick">
+        <color rgb="FF181818"/>
+      </left>
+      <right/>
+      <top style="thick">
+        <color rgb="FF181818"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1294,11 +1697,90 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="33" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="22" fillId="0" borderId="23" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="21" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="22" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1653,7 +2135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C594"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -8202,7 +8684,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B170"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -9319,10 +9801,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
@@ -9665,4 +10147,323 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{366D8DBA-A301-4C7A-946A-62B3B7943915}">
+  <dimension ref="A1:S8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="8.7265625" customWidth="1"/>
+    <col min="3" max="3" width="13.36328125" customWidth="1"/>
+    <col min="5" max="5" width="11.36328125" customWidth="1"/>
+    <col min="7" max="7" width="11.36328125" customWidth="1"/>
+    <col min="9" max="9" width="12.81640625" customWidth="1"/>
+    <col min="11" max="11" width="14.453125" customWidth="1"/>
+    <col min="13" max="13" width="11.90625" customWidth="1"/>
+    <col min="15" max="15" width="12" customWidth="1"/>
+    <col min="19" max="19" width="14.08984375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" ht="24.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>263</v>
+      </c>
+      <c r="C1" s="7"/>
+      <c r="D1" s="6" t="s">
+        <v>264</v>
+      </c>
+      <c r="E1" s="7"/>
+      <c r="F1" s="6" t="s">
+        <v>265</v>
+      </c>
+      <c r="G1" s="7"/>
+      <c r="H1" s="6" t="s">
+        <v>266</v>
+      </c>
+      <c r="I1" s="7"/>
+      <c r="J1" s="8" t="s">
+        <v>275</v>
+      </c>
+      <c r="K1" s="9"/>
+      <c r="L1" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="M1" s="11"/>
+      <c r="N1" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="O1" s="11"/>
+      <c r="P1" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="12" t="s">
+        <v>274</v>
+      </c>
+      <c r="S1" s="13"/>
+    </row>
+    <row r="2" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="B2" s="16">
+        <v>9</v>
+      </c>
+      <c r="C2" s="17">
+        <v>4.9500000000000003E-7</v>
+      </c>
+      <c r="D2" s="16">
+        <v>15</v>
+      </c>
+      <c r="E2" s="17">
+        <v>6.6800000000000005E-11</v>
+      </c>
+      <c r="F2" s="16">
+        <v>16</v>
+      </c>
+      <c r="G2" s="17">
+        <v>7.2799999999999997E-12</v>
+      </c>
+      <c r="H2" s="16">
+        <v>14</v>
+      </c>
+      <c r="I2" s="17">
+        <v>3.1599999999999999E-11</v>
+      </c>
+      <c r="J2" s="18">
+        <v>3</v>
+      </c>
+      <c r="K2" s="19">
+        <v>1.6699999999999999E-4</v>
+      </c>
+      <c r="L2" s="20">
+        <v>1</v>
+      </c>
+      <c r="M2" s="21">
+        <v>9.4999999999999998E-3</v>
+      </c>
+      <c r="N2" s="20">
+        <v>10</v>
+      </c>
+      <c r="O2" s="19">
+        <v>3.9300000000000001E-8</v>
+      </c>
+      <c r="P2" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q2" s="19">
+        <v>4.69E-6</v>
+      </c>
+      <c r="R2" s="22">
+        <v>4</v>
+      </c>
+      <c r="S2" s="23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="14" t="s">
+        <v>268</v>
+      </c>
+      <c r="B3" s="16">
+        <v>10</v>
+      </c>
+      <c r="C3" s="17">
+        <v>1.48E-8</v>
+      </c>
+      <c r="D3" s="16">
+        <v>14</v>
+      </c>
+      <c r="E3" s="17">
+        <v>2.1299999999999999E-10</v>
+      </c>
+      <c r="F3" s="16">
+        <v>16</v>
+      </c>
+      <c r="G3" s="17">
+        <v>1.33E-12</v>
+      </c>
+      <c r="H3" s="16">
+        <v>14</v>
+      </c>
+      <c r="I3" s="17">
+        <v>7.4E-12</v>
+      </c>
+      <c r="J3" s="18">
+        <v>2</v>
+      </c>
+      <c r="K3" s="21">
+        <v>2.5000000000000001E-3</v>
+      </c>
+      <c r="L3" s="20">
+        <v>1</v>
+      </c>
+      <c r="M3" s="21">
+        <v>8.0999999999999996E-3</v>
+      </c>
+      <c r="N3" s="20">
+        <v>10</v>
+      </c>
+      <c r="O3" s="19">
+        <v>1.48E-8</v>
+      </c>
+      <c r="P3" s="20">
+        <v>4</v>
+      </c>
+      <c r="Q3" s="19">
+        <v>5.8999999999999998E-5</v>
+      </c>
+      <c r="R3" s="22">
+        <v>4</v>
+      </c>
+      <c r="S3" s="23" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A4" s="14" t="s">
+        <v>269</v>
+      </c>
+      <c r="B4" s="16">
+        <v>12</v>
+      </c>
+      <c r="C4" s="17">
+        <v>4.7500000000000001E-10</v>
+      </c>
+      <c r="D4" s="16">
+        <v>14</v>
+      </c>
+      <c r="E4" s="17">
+        <v>3.1099999999999998E-9</v>
+      </c>
+      <c r="F4" s="16">
+        <v>16</v>
+      </c>
+      <c r="G4" s="17">
+        <v>3.3100000000000001E-11</v>
+      </c>
+      <c r="H4" s="16">
+        <v>14</v>
+      </c>
+      <c r="I4" s="17">
+        <v>1.16E-10</v>
+      </c>
+      <c r="J4" s="18">
+        <v>4</v>
+      </c>
+      <c r="K4" s="19">
+        <v>8.7399999999999993E-6</v>
+      </c>
+      <c r="L4" s="20">
+        <v>1</v>
+      </c>
+      <c r="M4" s="21">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="N4" s="20">
+        <v>10</v>
+      </c>
+      <c r="O4" s="19">
+        <v>9.5000000000000004E-8</v>
+      </c>
+      <c r="P4" s="20">
+        <v>5</v>
+      </c>
+      <c r="Q4" s="19">
+        <v>7.4699999999999996E-6</v>
+      </c>
+      <c r="R4" s="22">
+        <v>4</v>
+      </c>
+      <c r="S4" s="23" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A5" s="15" t="s">
+        <v>270</v>
+      </c>
+      <c r="B5" s="24">
+        <v>17</v>
+      </c>
+      <c r="C5" s="25">
+        <v>8.5300000000000005E-11</v>
+      </c>
+      <c r="D5" s="24">
+        <v>23</v>
+      </c>
+      <c r="E5" s="25">
+        <v>4.7700000000000001E-12</v>
+      </c>
+      <c r="F5" s="24">
+        <v>26</v>
+      </c>
+      <c r="G5" s="25">
+        <v>1.04E-14</v>
+      </c>
+      <c r="H5" s="24">
+        <v>21</v>
+      </c>
+      <c r="I5" s="25">
+        <v>2.3900000000000001E-12</v>
+      </c>
+      <c r="J5" s="26">
+        <v>5</v>
+      </c>
+      <c r="K5" s="27">
+        <v>1.5699999999999999E-5</v>
+      </c>
+      <c r="L5" s="28">
+        <v>3</v>
+      </c>
+      <c r="M5" s="29" t="s">
+        <v>279</v>
+      </c>
+      <c r="N5" s="28">
+        <v>14</v>
+      </c>
+      <c r="O5" s="27">
+        <v>7.5899999999999998E-8</v>
+      </c>
+      <c r="P5" s="28">
+        <v>7</v>
+      </c>
+      <c r="Q5" s="27">
+        <v>3.1499999999999999E-6</v>
+      </c>
+      <c r="R5" s="30">
+        <v>5</v>
+      </c>
+      <c r="S5" s="29" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="K8" s="4"/>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>